<commit_message>
[prof_attend_conference]: Update example file.
</commit_message>
<xml_diff>
--- a/public/Excel_example/prof/prof_attend_conference.xlsx
+++ b/public/Excel_example/prof/prof_attend_conference.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>姓名</t>
   </si>
@@ -41,6 +41,10 @@
   </si>
   <si>
     <t>所屬系所部門</t>
+  </si>
+  <si>
+    <t>發表論文名稱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -412,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -426,12 +430,12 @@
     <col min="4" max="4" width="47.75" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="13.625" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
     <col min="8" max="8" width="13.875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -451,12 +455,15 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>